<commit_message>
Handle the account data
</commit_message>
<xml_diff>
--- a/src/resource/account/financialindexdb.xlsx
+++ b/src/resource/account/financialindexdb.xlsx
@@ -41,10 +41,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>shareindices</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>摊薄每股收益(元)</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -172,10 +168,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>profitability</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>总资产利润率(%)</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -420,10 +412,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>growthability</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>主营业务收入增长率(%)</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -612,10 +600,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>debtcapitalstructure</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>流动比率</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -802,9 +786,6 @@
     <t>cash flow</t>
   </si>
   <si>
-    <t>cashflow</t>
-  </si>
-  <si>
     <t>经营现金净流量对销售收入比率(%)</t>
   </si>
   <si>
@@ -856,9 +837,6 @@
     <t>Other indicators</t>
   </si>
   <si>
-    <t>otherindicator</t>
-  </si>
-  <si>
     <t>短期股票投资(元)</t>
   </si>
   <si>
@@ -1046,6 +1024,24 @@
   </si>
   <si>
     <t>maxsize</t>
+  </si>
+  <si>
+    <t>fi_shareindex</t>
+  </si>
+  <si>
+    <t>fi_profitability</t>
+  </si>
+  <si>
+    <t>fi_growthability</t>
+  </si>
+  <si>
+    <t>fi_debtcapitalstructure</t>
+  </si>
+  <si>
+    <t>fi_cashflow</t>
+  </si>
+  <si>
+    <t>fi_otherindicator</t>
   </si>
 </sst>
 </file>
@@ -1427,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1446,27 +1442,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E2" s="10"/>
     </row>
@@ -1481,21 +1477,21 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -1509,178 +1505,178 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>287</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -1688,16 +1684,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E18">
         <v>10</v>
@@ -1705,16 +1701,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E19">
         <v>10</v>
@@ -1722,16 +1718,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E20">
         <v>10</v>
@@ -1739,16 +1735,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E21">
         <v>10</v>
@@ -1756,16 +1752,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1773,16 +1769,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1790,16 +1786,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E24">
         <v>10</v>
@@ -1807,16 +1803,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1824,16 +1820,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E26">
         <v>10</v>
@@ -1841,16 +1837,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E27">
         <v>10</v>
@@ -1858,16 +1854,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E28">
         <v>10</v>
@@ -1875,16 +1871,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1892,16 +1888,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1909,16 +1905,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E31">
         <v>10</v>
@@ -1926,16 +1922,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -1943,16 +1939,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -1960,16 +1956,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E34">
         <v>10</v>
@@ -1977,16 +1973,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E35">
         <v>10</v>
@@ -1994,16 +1990,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E36">
         <v>20</v>
@@ -2011,30 +2007,30 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>101</v>
+        <v>289</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E38">
         <v>10</v>
@@ -2042,16 +2038,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E39">
         <v>10</v>
@@ -2059,16 +2055,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E40">
         <v>10</v>
@@ -2076,16 +2072,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E41">
         <v>10</v>
@@ -2093,30 +2089,30 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D43" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E43">
         <v>10</v>
@@ -2124,16 +2120,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D44" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -2141,16 +2137,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E45">
         <v>10</v>
@@ -2158,16 +2154,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D46" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -2175,16 +2171,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E47">
         <v>10</v>
@@ -2192,16 +2188,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E48">
         <v>10</v>
@@ -2209,16 +2205,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D49" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E49">
         <v>10</v>
@@ -2226,16 +2222,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E50">
         <v>10</v>
@@ -2243,16 +2239,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E51">
         <v>10</v>
@@ -2260,16 +2256,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -2277,30 +2273,30 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>149</v>
+        <v>290</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E54">
         <v>10</v>
@@ -2308,16 +2304,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D55" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E55">
         <v>10</v>
@@ -2325,16 +2321,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B56" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D56" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E56">
         <v>10</v>
@@ -2342,16 +2338,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C57" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D57" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E57">
         <v>10</v>
@@ -2359,16 +2355,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C58" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D58" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E58">
         <v>10</v>
@@ -2376,16 +2372,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E59">
         <v>10</v>
@@ -2393,16 +2389,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D60" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E60">
         <v>10</v>
@@ -2410,16 +2406,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B61" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D61" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E61">
         <v>10</v>
@@ -2427,16 +2423,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E62">
         <v>10</v>
@@ -2444,16 +2440,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C63" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D63" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E63">
         <v>10</v>
@@ -2461,16 +2457,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B64" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D64" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E64">
         <v>10</v>
@@ -2478,16 +2474,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C65" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D65" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E65">
         <v>10</v>
@@ -2495,16 +2491,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B66" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C66" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D66" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E66">
         <v>10</v>
@@ -2512,16 +2508,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C67" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E67">
         <v>10</v>
@@ -2529,16 +2525,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C68" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D68" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E68">
         <v>10</v>
@@ -2546,16 +2542,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D69" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E69">
         <v>10</v>
@@ -2563,16 +2559,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B70" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E70">
         <v>10</v>
@@ -2580,16 +2576,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E71">
         <v>20</v>
@@ -2597,30 +2593,30 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="8" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>211</v>
+        <v>291</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B73" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E73">
         <v>10</v>
@@ -2628,16 +2624,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D74" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E74">
         <v>10</v>
@@ -2645,16 +2641,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C75" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D75" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E75">
         <v>10</v>
@@ -2662,16 +2658,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C76" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D76" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E76">
         <v>10</v>
@@ -2679,16 +2675,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B77" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C77" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E77">
         <v>10</v>
@@ -2696,30 +2692,30 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>229</v>
+        <v>292</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B79" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D79" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E79">
         <v>20</v>
@@ -2727,16 +2723,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B80" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C80" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D80" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E80">
         <v>20</v>
@@ -2744,16 +2740,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B81" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D81" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E81">
         <v>20</v>
@@ -2761,16 +2757,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B82" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D82" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E82">
         <v>20</v>
@@ -2778,16 +2774,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B83" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C83" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D83" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E83">
         <v>20</v>
@@ -2795,16 +2791,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B84" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C84" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D84" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E84">
         <v>20</v>
@@ -2812,16 +2808,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B85" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C85" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D85" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E85">
         <v>20</v>
@@ -2829,16 +2825,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B86" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C86" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E86">
         <v>20</v>
@@ -2846,16 +2842,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C87" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D87" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E87">
         <v>20</v>
@@ -2863,16 +2859,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B88" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C88" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D88" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E88">
         <v>20</v>
@@ -2880,16 +2876,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B89" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C89" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D89" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E89">
         <v>20</v>
@@ -2897,16 +2893,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B90" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C90" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D90" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E90">
         <v>20</v>
@@ -2914,16 +2910,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B91" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C91" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D91" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E91">
         <v>20</v>
@@ -2931,16 +2927,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B92" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C92" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D92" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E92">
         <v>20</v>
@@ -2948,16 +2944,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B93" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C93" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D93" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E93">
         <v>20</v>
@@ -2965,16 +2961,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B94" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C94" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D94" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E94">
         <v>20</v>
@@ -2982,16 +2978,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
+        <v>272</v>
+      </c>
+      <c r="B95" t="s">
+        <v>273</v>
+      </c>
+      <c r="C95" t="s">
+        <v>274</v>
+      </c>
+      <c r="D95" t="s">
         <v>278</v>
-      </c>
-      <c r="B95" t="s">
-        <v>279</v>
-      </c>
-      <c r="C95" t="s">
-        <v>280</v>
-      </c>
-      <c r="D95" t="s">
-        <v>284</v>
       </c>
       <c r="E95">
         <v>20</v>
@@ -2999,16 +2995,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B96" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C96" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D96" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E96">
         <v>20</v>

</xml_diff>